<commit_message>
chg: Updated Ordnance information with amount of Mavericks
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t xml:space="preserve"> GBU-54: 20</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>F/A-18, F-16, F-14</t>
+  </si>
+  <si>
+    <t>AGM-65 (all types)</t>
   </si>
 </sst>
 </file>
@@ -205,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -431,11 +434,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -507,6 +523,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,7 +928,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1405,39 +1427,65 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A17" s="7" t="s">
+    <row r="17" spans="1:18">
+      <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="20">
         <v>15</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23">
+      <c r="D17" s="20"/>
+      <c r="E17" s="20">
         <v>5</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="19">
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="20"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="20"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
-      <c r="L18" s="1"/>
+    <row r="18" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="23">
+        <v>50</v>
+      </c>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="19">
+        <f>E18-SUM(F18:Q18)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="19" spans="1:18">
       <c r="L19" s="1"/>
@@ -1455,9 +1503,10 @@
       <c r="L23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="O1:Q2"/>
+    <mergeCell ref="C18:D18"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Update ordnance +  weather forecast next 3 ATO days
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t xml:space="preserve"> GBU-54: 20</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>AGM-65 (all types)</t>
+  </si>
+  <si>
+    <t>Fuel tanks (all types)</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -447,11 +450,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -506,12 +520,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -528,6 +536,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -544,15 +572,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>828674</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -561,8 +589,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="333374" y="3552825"/>
-          <a:ext cx="8429625" cy="2486025"/>
+          <a:off x="304799" y="3952875"/>
+          <a:ext cx="8429625" cy="2181225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -928,7 +956,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -955,13 +983,13 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="26" t="s">
-        <v>4</v>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="24" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -981,10 +1009,10 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="25"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
@@ -1381,7 +1409,9 @@
       <c r="E15" s="20">
         <v>4</v>
       </c>
-      <c r="F15" s="20"/>
+      <c r="F15" s="20">
+        <v>4</v>
+      </c>
       <c r="G15" s="20"/>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
@@ -1395,7 +1425,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="18">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1458,37 +1488,65 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="15.75" thickBot="1">
-      <c r="A18" s="7" t="s">
+    <row r="18" spans="1:18">
+      <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="30"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="23">
+      <c r="D18" s="30"/>
+      <c r="E18" s="35">
         <v>50</v>
       </c>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="19">
+      <c r="F18" s="35">
+        <v>5</v>
+      </c>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="35"/>
+      <c r="N18" s="35"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="23">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:18">
-      <c r="L19" s="1"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="33"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="19">
+        <f>F19-SUM(G19:Q19)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="20" spans="1:18">
       <c r="L20" s="1"/>
@@ -1503,10 +1561,11 @@
       <c r="L23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="R1:R2"/>
     <mergeCell ref="O1:Q2"/>
     <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:E19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
chg: Added SPINS version 2 and updated ordnance
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEFB465-EF28-4531-BCA2-BB0ED6E5465D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="18495" windowHeight="11700"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -153,8 +166,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -465,7 +478,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -486,11 +499,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -518,30 +531,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -549,13 +538,28 @@
       <alignment horizontal="left" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -564,6 +568,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -584,7 +596,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TekstSylinder 1"/>
+        <xdr:cNvPr id="2" name="TekstSylinder 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -711,7 +729,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -743,9 +761,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -777,6 +813,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -952,23 +1006,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="R1" sqref="R1:R2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="17" width="5.28515625" customWidth="1"/>
-    <col min="18" max="18" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.109375" customWidth="1"/>
+    <col min="4" max="17" width="5.33203125" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -983,16 +1037,16 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="24" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="27" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="14" t="s">
@@ -1009,12 +1063,12 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="25"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1">
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="28"/>
+    </row>
+    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
@@ -1070,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -1099,7 +1153,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1128,7 +1182,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1157,7 +1211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -1186,7 +1240,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -1215,7 +1269,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>40</v>
       </c>
@@ -1228,7 +1282,9 @@
       <c r="D9" s="20"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
-      <c r="G9" s="20"/>
+      <c r="G9" s="20">
+        <v>2</v>
+      </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
@@ -1241,10 +1297,10 @@
       <c r="Q9" s="21"/>
       <c r="R9" s="18">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -1273,7 +1329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1302,7 +1358,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1319,7 +1375,9 @@
         <v>8</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="4">
+        <v>4</v>
+      </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1332,10 +1390,10 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="18">
         <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1364,7 +1422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
@@ -1393,7 +1451,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1428,7 +1486,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -1457,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
@@ -1488,76 +1546,76 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="35">
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="4">
         <v>50</v>
       </c>
-      <c r="F18" s="35">
+      <c r="F18" s="4">
         <v>5</v>
       </c>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="37"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1">
+    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="29"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="23">
         <v>50</v>
       </c>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="33"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="34"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="26"/>
       <c r="R19" s="19">
         <f>F19-SUM(G19:Q19)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="L23" s="1"/>
     </row>
   </sheetData>
@@ -1574,12 +1632,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1587,12 +1645,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
chg: Updated ordnance status + weather for D3.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEFB465-EF28-4531-BCA2-BB0ED6E5465D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -166,8 +165,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -599,7 +598,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -729,7 +728,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -761,27 +760,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -813,24 +794,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1006,23 +969,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" customWidth="1"/>
-    <col min="4" max="17" width="5.33203125" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="17" width="5.28515625" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1043,10 +1006,10 @@
       <c r="P1" s="29"/>
       <c r="Q1" s="29"/>
       <c r="R1" s="27" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="14" t="s">
@@ -1068,7 +1031,7 @@
       <c r="Q2" s="30"/>
       <c r="R2" s="28"/>
     </row>
-    <row r="3" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
@@ -1124,7 +1087,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -1153,7 +1116,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1182,7 +1145,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1211,7 +1174,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -1240,7 +1203,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -1269,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18">
       <c r="A9" s="6" t="s">
         <v>40</v>
       </c>
@@ -1300,7 +1263,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -1329,7 +1292,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1358,7 +1321,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1378,7 +1341,9 @@
       <c r="G12" s="4">
         <v>4</v>
       </c>
-      <c r="H12" s="4"/>
+      <c r="H12" s="4">
+        <v>3</v>
+      </c>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -1390,10 +1355,10 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="18">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1372,9 @@
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
+      <c r="H13" s="20">
+        <v>6</v>
+      </c>
       <c r="I13" s="20"/>
       <c r="J13" s="20"/>
       <c r="K13" s="20"/>
@@ -1419,10 +1386,10 @@
       <c r="Q13" s="21"/>
       <c r="R13" s="18">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
@@ -1451,7 +1418,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1471,7 +1438,9 @@
         <v>4</v>
       </c>
       <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="H15" s="20">
+        <v>2</v>
+      </c>
       <c r="I15" s="20"/>
       <c r="J15" s="20"/>
       <c r="K15" s="20"/>
@@ -1483,10 +1452,10 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="18">
         <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -1515,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18">
       <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
@@ -1546,7 +1515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1562,7 +1531,9 @@
         <v>5</v>
       </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="4">
+        <v>6</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
@@ -1574,10 +1545,10 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1591,7 +1562,9 @@
         <v>50</v>
       </c>
       <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="H19" s="24">
+        <v>8</v>
+      </c>
       <c r="I19" s="24"/>
       <c r="J19" s="24"/>
       <c r="K19" s="24"/>
@@ -1603,19 +1576,19 @@
       <c r="Q19" s="26"/>
       <c r="R19" s="19">
         <f>F19-SUM(G19:Q19)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18">
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18">
       <c r="L23" s="1"/>
     </row>
   </sheetData>
@@ -1632,12 +1605,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1645,12 +1618,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
chg: Updated ordnance overview and updated weather for D4.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -477,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -532,11 +532,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -973,7 +974,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1000,13 +1001,13 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
-      <c r="O1" s="29" t="s">
+      <c r="O1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="27" t="s">
-        <v>15</v>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="26" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1026,10 +1027,10 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="30"/>
-      <c r="R2" s="28"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="27"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
@@ -1101,7 +1102,9 @@
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4">
+        <v>3</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -1113,7 +1116,7 @@
       <c r="Q4" s="15"/>
       <c r="R4" s="17">
         <f>C4-SUM(D4:Q4)</f>
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -1344,7 +1347,9 @@
       <c r="H12" s="4">
         <v>3</v>
       </c>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4">
+        <v>8</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
@@ -1355,7 +1360,7 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="18">
         <f t="shared" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1404,7 +1409,9 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4">
+        <v>8</v>
+      </c>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="5"/>
@@ -1415,7 +1422,7 @@
       <c r="Q14" s="15"/>
       <c r="R14" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1522,8 +1529,8 @@
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
       <c r="E18" s="4">
         <v>50</v>
       </c>
@@ -1534,7 +1541,9 @@
       <c r="H18" s="4">
         <v>6</v>
       </c>
-      <c r="I18" s="4"/>
+      <c r="I18" s="4">
+        <v>8</v>
+      </c>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="5"/>
@@ -1545,7 +1554,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1">
@@ -1555,28 +1564,30 @@
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="23">
         <v>50</v>
       </c>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24">
+      <c r="G19" s="23"/>
+      <c r="H19" s="23">
         <v>8</v>
       </c>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="25"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="26"/>
+      <c r="I19" s="23">
+        <v>2</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="25"/>
       <c r="R19" s="19">
         <f>F19-SUM(G19:Q19)</f>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:18">

</xml_diff>

<commit_message>
chg: Updates to ordnance from D4.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -599,7 +599,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -974,7 +974,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1007,7 +1007,7 @@
       <c r="P1" s="28"/>
       <c r="Q1" s="28"/>
       <c r="R1" s="26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1350,7 +1350,9 @@
       <c r="I12" s="4">
         <v>8</v>
       </c>
-      <c r="J12" s="4"/>
+      <c r="J12" s="4">
+        <v>2</v>
+      </c>
       <c r="K12" s="4"/>
       <c r="L12" s="5"/>
       <c r="M12" s="4"/>
@@ -1360,7 +1362,7 @@
       <c r="Q12" s="15"/>
       <c r="R12" s="18">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1449,7 +1451,9 @@
         <v>2</v>
       </c>
       <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
+      <c r="J15" s="20">
+        <v>9</v>
+      </c>
       <c r="K15" s="20"/>
       <c r="L15" s="22"/>
       <c r="M15" s="20"/>
@@ -1459,7 +1463,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="18">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1544,7 +1548,9 @@
       <c r="I18" s="4">
         <v>8</v>
       </c>
-      <c r="J18" s="4"/>
+      <c r="J18" s="4">
+        <v>3</v>
+      </c>
       <c r="K18" s="4"/>
       <c r="L18" s="5"/>
       <c r="M18" s="4"/>
@@ -1554,7 +1560,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1">
@@ -1577,7 +1583,9 @@
       <c r="I19" s="23">
         <v>2</v>
       </c>
-      <c r="J19" s="23"/>
+      <c r="J19" s="23">
+        <v>4</v>
+      </c>
       <c r="K19" s="23"/>
       <c r="L19" s="24"/>
       <c r="M19" s="23"/>
@@ -1587,7 +1595,7 @@
       <c r="Q19" s="25"/>
       <c r="R19" s="19">
         <f>F19-SUM(G19:Q19)</f>
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:18">

</xml_diff>

<commit_message>
chg: Added JFC D&G D5, VID Intsum D4, SOCC Intrep D4, Updated ordnance
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +192,19 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -477,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -560,6 +573,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -599,7 +618,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -974,7 +993,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="R1" sqref="R1:R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1007,7 +1026,7 @@
       <c r="P1" s="28"/>
       <c r="Q1" s="28"/>
       <c r="R1" s="26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1230,7 +1249,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="18">
+      <c r="R8" s="35">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1353,16 +1372,18 @@
       <c r="J12" s="4">
         <v>2</v>
       </c>
-      <c r="K12" s="4"/>
+      <c r="K12" s="4">
+        <v>6</v>
+      </c>
       <c r="L12" s="5"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="15"/>
-      <c r="R12" s="18">
+      <c r="R12" s="34">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1415,16 +1436,18 @@
         <v>8</v>
       </c>
       <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
+      <c r="K14" s="4">
+        <v>4</v>
+      </c>
       <c r="L14" s="5"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="15"/>
-      <c r="R14" s="18">
+      <c r="R14" s="34">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:18">
@@ -1454,7 +1477,9 @@
       <c r="J15" s="20">
         <v>9</v>
       </c>
-      <c r="K15" s="20"/>
+      <c r="K15" s="20">
+        <v>10</v>
+      </c>
       <c r="L15" s="22"/>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
@@ -1463,7 +1488,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="18">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1551,7 +1576,9 @@
       <c r="J18" s="4">
         <v>3</v>
       </c>
-      <c r="K18" s="4"/>
+      <c r="K18" s="4">
+        <v>4</v>
+      </c>
       <c r="L18" s="5"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -1560,7 +1587,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1">
@@ -1586,7 +1613,9 @@
       <c r="J19" s="23">
         <v>4</v>
       </c>
-      <c r="K19" s="23"/>
+      <c r="K19" s="23">
+        <v>6</v>
+      </c>
       <c r="L19" s="24"/>
       <c r="M19" s="23"/>
       <c r="N19" s="23"/>
@@ -1595,7 +1624,7 @@
       <c r="Q19" s="25"/>
       <c r="R19" s="19">
         <f>F19-SUM(G19:Q19)</f>
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:18">

</xml_diff>

<commit_message>
chg: Updated spent ordnance on D5.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -551,6 +551,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -573,12 +579,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -618,7 +618,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -993,7 +993,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:R2"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1020,13 +1020,13 @@
       <c r="L1" s="10"/>
       <c r="M1" s="10"/>
       <c r="N1" s="10"/>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="26" t="s">
-        <v>17</v>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="28" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1046,10 +1046,10 @@
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="27"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="29"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1">
       <c r="A3" s="13" t="s">
@@ -1249,7 +1249,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
       <c r="Q8" s="15"/>
-      <c r="R8" s="35">
+      <c r="R8" s="27">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -1332,7 +1332,9 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20"/>
-      <c r="L11" s="22"/>
+      <c r="L11" s="20">
+        <v>6</v>
+      </c>
       <c r="M11" s="20"/>
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
@@ -1340,7 +1342,7 @@
       <c r="Q11" s="21"/>
       <c r="R11" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1381,7 +1383,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
       <c r="Q12" s="15"/>
-      <c r="R12" s="34">
+      <c r="R12" s="26">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1445,7 +1447,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
       <c r="Q14" s="15"/>
-      <c r="R14" s="34">
+      <c r="R14" s="26">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1480,7 +1482,9 @@
       <c r="K15" s="20">
         <v>10</v>
       </c>
-      <c r="L15" s="22"/>
+      <c r="L15" s="20">
+        <v>2</v>
+      </c>
       <c r="M15" s="20"/>
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
@@ -1488,7 +1492,7 @@
       <c r="Q15" s="21"/>
       <c r="R15" s="18">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1558,8 +1562,8 @@
       <c r="B18" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="4">
         <v>50</v>
       </c>
@@ -1579,7 +1583,9 @@
       <c r="K18" s="4">
         <v>4</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="4">
+        <v>2</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1587,7 +1593,7 @@
       <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1">
@@ -1597,9 +1603,9 @@
       <c r="B19" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="23">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
chg: Updates for 6.1 (CJTF D&G, Weather, ordnance, VID Intsum)
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -618,7 +618,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -993,7 +993,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1026,7 +1026,7 @@
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -1485,14 +1485,16 @@
       <c r="L15" s="20">
         <v>2</v>
       </c>
-      <c r="M15" s="20"/>
+      <c r="M15" s="20">
+        <v>8</v>
+      </c>
       <c r="N15" s="20"/>
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
-      <c r="R15" s="18">
+      <c r="R15" s="26">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1586,14 +1588,16 @@
       <c r="L18" s="4">
         <v>2</v>
       </c>
-      <c r="M18" s="4"/>
+      <c r="M18" s="4">
+        <v>3</v>
+      </c>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="18">
         <f>E18-SUM(F18:Q18)</f>
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
chg: Updated available ordnance
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCEE7ABA-A593-4AD1-B1C3-5CB4CE7E3304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="Ark2" sheetId="2" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -21,6 +22,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -165,8 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -618,7 +620,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -748,7 +750,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,9 +782,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -814,6 +834,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -989,14 +1027,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
@@ -1005,7 +1043,7 @@
     <col min="18" max="18" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1026,10 +1064,10 @@
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
       <c r="R1" s="28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="14" t="s">
@@ -1051,7 +1089,7 @@
       <c r="Q2" s="31"/>
       <c r="R2" s="29"/>
     </row>
-    <row r="3" spans="1:18" ht="15.75" thickBot="1">
+    <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1145,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -1138,7 +1176,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>29</v>
       </c>
@@ -1167,7 +1205,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
@@ -1196,7 +1234,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
@@ -1225,7 +1263,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>32</v>
       </c>
@@ -1254,7 +1292,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>40</v>
       </c>
@@ -1285,7 +1323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
@@ -1314,7 +1352,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1345,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1388,7 +1426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>0</v>
       </c>
@@ -1419,7 +1457,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>36</v>
       </c>
@@ -1452,7 +1490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -1488,16 +1526,18 @@
       <c r="M15" s="20">
         <v>8</v>
       </c>
-      <c r="N15" s="20"/>
+      <c r="N15" s="20">
+        <v>2</v>
+      </c>
       <c r="O15" s="20"/>
       <c r="P15" s="20"/>
       <c r="Q15" s="21"/>
       <c r="R15" s="26">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>38</v>
       </c>
@@ -1526,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
@@ -1557,7 +1597,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>42</v>
       </c>
@@ -1591,16 +1631,18 @@
       <c r="M18" s="4">
         <v>3</v>
       </c>
-      <c r="N18" s="4"/>
+      <c r="N18" s="4">
+        <v>16</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
       <c r="Q18" s="15"/>
-      <c r="R18" s="18">
+      <c r="R18" s="26">
         <f>E18-SUM(F18:Q18)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="15.75" thickBot="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1637,16 +1679,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:18">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:18">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="L23" s="1"/>
     </row>
   </sheetData>
@@ -1657,18 +1699,18 @@
     <mergeCell ref="C19:E19"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -1676,12 +1718,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
chg: Added CJTF D&G for D8, VID Intsum from D7, updated weather for D8.1, updated ordnance for D8
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>D0</t>
   </si>
@@ -167,6 +167,9 @@
   </si>
   <si>
     <t xml:space="preserve"> GBU-54</t>
+  </si>
+  <si>
+    <t>D8.1</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>828674</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -659,7 +662,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1031,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1045,12 +1048,15 @@
     <col min="6" max="6" width="4.5703125" customWidth="1"/>
     <col min="7" max="7" width="4.42578125" customWidth="1"/>
     <col min="8" max="8" width="3.85546875" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" customWidth="1"/>
-    <col min="10" max="19" width="5.28515625" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" customWidth="1"/>
+    <col min="9" max="11" width="4.5703125" customWidth="1"/>
+    <col min="12" max="12" width="4.42578125" customWidth="1"/>
+    <col min="13" max="13" width="4.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5" customWidth="1"/>
+    <col min="15" max="20" width="5.28515625" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" customHeight="1">
+    <row r="1" spans="1:21" ht="15" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
       <c r="C1" s="42" t="s">
@@ -1078,11 +1084,12 @@
       </c>
       <c r="R1" s="40"/>
       <c r="S1" s="40"/>
-      <c r="T1" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="69.75" customHeight="1">
+      <c r="T1" s="40"/>
+      <c r="U1" s="38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="69.75" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="34"/>
       <c r="C2" s="43"/>
@@ -1102,9 +1109,10 @@
       <c r="Q2" s="41"/>
       <c r="R2" s="41"/>
       <c r="S2" s="41"/>
-      <c r="T2" s="39"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.75" thickBot="1">
+      <c r="T2" s="41"/>
+      <c r="U2" s="39"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -1158,11 +1166,14 @@
       <c r="S3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="12" t="s">
+      <c r="T3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="U3" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1190,12 +1201,13 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
       <c r="S4" s="11"/>
-      <c r="T4" s="19">
-        <f t="shared" ref="T4:T11" si="0">SUM(C4:E4)-SUM(F4:S4)</f>
+      <c r="T4" s="11"/>
+      <c r="U4" s="19">
+        <f>SUM(C4:E4)-SUM(F4:T4)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -1221,12 +1233,13 @@
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
       <c r="S5" s="14"/>
-      <c r="T5" s="19">
-        <f t="shared" si="0"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="19">
+        <f>SUM(C5:E5)-SUM(F5:T5)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -1252,12 +1265,13 @@
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
       <c r="S6" s="11"/>
-      <c r="T6" s="19">
-        <f t="shared" si="0"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="19">
+        <f>SUM(C6:E6)-SUM(F6:T6)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1285,12 +1299,13 @@
       </c>
       <c r="R7" s="13"/>
       <c r="S7" s="14"/>
-      <c r="T7" s="19">
-        <f t="shared" si="0"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="19">
+        <f>SUM(C7:E7)-SUM(F7:T7)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1316,12 +1331,13 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
       <c r="S8" s="11"/>
-      <c r="T8" s="19">
-        <f t="shared" si="0"/>
+      <c r="T8" s="11"/>
+      <c r="U8" s="19">
+        <f>SUM(C8:E8)-SUM(F8:T8)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -1349,12 +1365,13 @@
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
       <c r="S9" s="14"/>
-      <c r="T9" s="19">
-        <f t="shared" si="0"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="19">
+        <f>SUM(C9:E9)-SUM(F9:T9)</f>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1380,12 +1397,13 @@
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
       <c r="S10" s="11"/>
-      <c r="T10" s="19">
-        <f t="shared" si="0"/>
+      <c r="T10" s="11"/>
+      <c r="U10" s="19">
+        <f>SUM(C10:E10)-SUM(F10:T10)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -1413,12 +1431,13 @@
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
       <c r="S11" s="14"/>
-      <c r="T11" s="19">
-        <f t="shared" si="0"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="19">
+        <f>SUM(C11:E11)-SUM(F11:T11)</f>
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1429,7 +1448,7 @@
         <v>50</v>
       </c>
       <c r="D12" s="27">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E12" s="27"/>
       <c r="F12" s="24">
@@ -1461,13 +1480,16 @@
       <c r="R12" s="3">
         <v>7</v>
       </c>
-      <c r="S12" s="11"/>
-      <c r="T12" s="19">
-        <f>SUM(C12:E12)-SUM(F12:S12)</f>
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="S12" s="11">
+        <v>4</v>
+      </c>
+      <c r="T12" s="11"/>
+      <c r="U12" s="19">
+        <f>SUM(C12:E12)-SUM(F12:T12)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="5" t="s">
         <v>45</v>
       </c>
@@ -1496,13 +1518,16 @@
         <v>5</v>
       </c>
       <c r="R13" s="13"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="19">
-        <f t="shared" ref="T13:T19" si="1">SUM(C13:E13)-SUM(F13:S13)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="S13" s="14">
+        <v>4</v>
+      </c>
+      <c r="T13" s="14"/>
+      <c r="U13" s="19">
+        <f>SUM(C13:E13)-SUM(F13:T13)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
@@ -1532,12 +1557,13 @@
       <c r="Q14" s="3"/>
       <c r="R14" s="3"/>
       <c r="S14" s="11"/>
-      <c r="T14" s="19">
-        <f>SUM(C14:E14)-SUM(F14:S14)</f>
+      <c r="T14" s="11"/>
+      <c r="U14" s="19">
+        <f>SUM(C14:E14)-SUM(F14:T14)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -1547,7 +1573,9 @@
       <c r="C15" s="28">
         <v>50</v>
       </c>
-      <c r="D15" s="28"/>
+      <c r="D15" s="28">
+        <v>50</v>
+      </c>
       <c r="E15" s="28"/>
       <c r="F15" s="25">
         <v>6</v>
@@ -1582,13 +1610,16 @@
         <v>1</v>
       </c>
       <c r="R15" s="13"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="19">
-        <f t="shared" si="1"/>
+      <c r="S15" s="14">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="T15" s="14"/>
+      <c r="U15" s="19">
+        <f>SUM(C15:E15)-SUM(F15:T15)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -1614,12 +1645,13 @@
       <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="11"/>
-      <c r="T16" s="19">
-        <f t="shared" si="1"/>
+      <c r="T16" s="11"/>
+      <c r="U16" s="19">
+        <f>SUM(C16:E16)-SUM(F16:T16)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:21">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -1647,12 +1679,13 @@
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
       <c r="S17" s="14"/>
-      <c r="T17" s="19">
-        <f t="shared" si="1"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="19">
+        <f>SUM(C17:E17)-SUM(F17:T17)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:21">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1663,7 +1696,7 @@
         <v>50</v>
       </c>
       <c r="D18" s="29">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="26"/>
@@ -1699,13 +1732,16 @@
       <c r="R18" s="3">
         <v>2</v>
       </c>
-      <c r="S18" s="11"/>
-      <c r="T18" s="19">
-        <f t="shared" si="1"/>
+      <c r="S18" s="11">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" ht="15.75" thickBot="1">
+      <c r="T18" s="11"/>
+      <c r="U18" s="19">
+        <f>SUM(C18:E18)-SUM(F18:T18)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1741,27 +1777,28 @@
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
       <c r="S19" s="18"/>
-      <c r="T19" s="36">
-        <f t="shared" si="1"/>
+      <c r="T19" s="18"/>
+      <c r="U19" s="36">
+        <f>SUM(C19:E19)-SUM(F19:T19)</f>
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:21">
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:21">
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:21">
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:21">
       <c r="N23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="Q1:S2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="Q1:T2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>

</xml_diff>

<commit_message>
chg: Updated weather and time for D8.2. Updated ordnance for D8.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -662,7 +662,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1086,7 +1086,7 @@
       <c r="S1" s="40"/>
       <c r="T1" s="40"/>
       <c r="U1" s="38" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="69.75" customHeight="1">
@@ -1203,7 +1203,7 @@
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="19">
-        <f>SUM(C4:E4)-SUM(F4:T4)</f>
+        <f t="shared" ref="U4:U19" si="0">SUM(C4:E4)-SUM(F4:T4)</f>
         <v>47</v>
       </c>
     </row>
@@ -1235,7 +1235,7 @@
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
       <c r="U5" s="19">
-        <f>SUM(C5:E5)-SUM(F5:T5)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1267,7 +1267,7 @@
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="19">
-        <f>SUM(C6:E6)-SUM(F6:T6)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1301,7 +1301,7 @@
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
       <c r="U7" s="19">
-        <f>SUM(C7:E7)-SUM(F7:T7)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -1333,7 +1333,7 @@
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
       <c r="U8" s="19">
-        <f>SUM(C8:E8)-SUM(F8:T8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1365,10 +1365,12 @@
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
       <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
+      <c r="T9" s="14">
+        <v>2</v>
+      </c>
       <c r="U9" s="19">
-        <f>SUM(C9:E9)-SUM(F9:T9)</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1399,7 +1401,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
       <c r="U10" s="19">
-        <f>SUM(C10:E10)-SUM(F10:T10)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
@@ -1433,7 +1435,7 @@
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
       <c r="U11" s="19">
-        <f>SUM(C11:E11)-SUM(F11:T11)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -1485,7 +1487,7 @@
       </c>
       <c r="T12" s="11"/>
       <c r="U12" s="19">
-        <f>SUM(C12:E12)-SUM(F12:T12)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
     </row>
@@ -1523,7 +1525,7 @@
       </c>
       <c r="T13" s="14"/>
       <c r="U13" s="19">
-        <f>SUM(C13:E13)-SUM(F13:T13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
@@ -1559,7 +1561,7 @@
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
       <c r="U14" s="19">
-        <f>SUM(C14:E14)-SUM(F14:T14)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -1615,7 +1617,7 @@
       </c>
       <c r="T15" s="14"/>
       <c r="U15" s="19">
-        <f>SUM(C15:E15)-SUM(F15:T15)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -1647,7 +1649,7 @@
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
       <c r="U16" s="19">
-        <f>SUM(C16:E16)-SUM(F16:T16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1681,7 +1683,7 @@
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
       <c r="U17" s="19">
-        <f>SUM(C17:E17)-SUM(F17:T17)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1735,10 +1737,12 @@
       <c r="S18" s="11">
         <v>9</v>
       </c>
-      <c r="T18" s="11"/>
+      <c r="T18" s="11">
+        <v>2</v>
+      </c>
       <c r="U18" s="19">
-        <f>SUM(C18:E18)-SUM(F18:T18)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="15.75" thickBot="1">
@@ -1779,7 +1783,7 @@
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
       <c r="U19" s="36">
-        <f>SUM(C19:E19)-SUM(F19:T19)</f>
+        <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chg: Updated ordnance for D9
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>D0</t>
   </si>
@@ -170,13 +170,16 @@
   </si>
   <si>
     <t>D8.1</t>
+  </si>
+  <si>
+    <t>D8.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,6 +215,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -508,7 +518,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -624,6 +634,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,7 +665,7 @@
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>828674</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -662,7 +675,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1034,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1052,11 +1065,11 @@
     <col min="12" max="12" width="4.42578125" customWidth="1"/>
     <col min="13" max="13" width="4.7109375" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
-    <col min="15" max="20" width="5.28515625" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" customWidth="1"/>
+    <col min="15" max="21" width="5.28515625" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" customHeight="1">
+    <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
       <c r="C1" s="42" t="s">
@@ -1085,11 +1098,12 @@
       <c r="R1" s="40"/>
       <c r="S1" s="40"/>
       <c r="T1" s="40"/>
-      <c r="U1" s="38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="69.75" customHeight="1">
+      <c r="U1" s="40"/>
+      <c r="V1" s="38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="69.75" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="34"/>
       <c r="C2" s="43"/>
@@ -1110,9 +1124,10 @@
       <c r="R2" s="41"/>
       <c r="S2" s="41"/>
       <c r="T2" s="41"/>
-      <c r="U2" s="39"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1">
+      <c r="U2" s="41"/>
+      <c r="V2" s="39"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
       <c r="A3" s="10" t="s">
         <v>24</v>
       </c>
@@ -1169,11 +1184,14 @@
       <c r="T3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="U3" s="12" t="s">
+      <c r="U3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" s="5" t="s">
         <v>27</v>
       </c>
@@ -1202,12 +1220,13 @@
       <c r="R4" s="3"/>
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
-      <c r="U4" s="19">
-        <f t="shared" ref="U4:U19" si="0">SUM(C4:E4)-SUM(F4:T4)</f>
+      <c r="U4" s="11"/>
+      <c r="V4" s="19">
+        <f t="shared" ref="V4:V19" si="0">SUM(C4:E4)-SUM(F4:U4)</f>
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" s="5" t="s">
         <v>28</v>
       </c>
@@ -1234,12 +1253,13 @@
       <c r="R5" s="13"/>
       <c r="S5" s="14"/>
       <c r="T5" s="14"/>
-      <c r="U5" s="19">
+      <c r="U5" s="14"/>
+      <c r="V5" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
@@ -1266,12 +1286,13 @@
       <c r="R6" s="3"/>
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
-      <c r="U6" s="19">
+      <c r="U6" s="11"/>
+      <c r="V6" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1300,12 +1321,13 @@
       <c r="R7" s="13"/>
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
-      <c r="U7" s="19">
+      <c r="U7" s="14"/>
+      <c r="V7" s="19">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1332,12 +1354,13 @@
       <c r="R8" s="3"/>
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
-      <c r="U8" s="19">
+      <c r="U8" s="11"/>
+      <c r="V8" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -1368,12 +1391,13 @@
       <c r="T9" s="14">
         <v>2</v>
       </c>
-      <c r="U9" s="19">
+      <c r="U9" s="14"/>
+      <c r="V9" s="19">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" s="5" t="s">
         <v>32</v>
       </c>
@@ -1400,12 +1424,13 @@
       <c r="R10" s="3"/>
       <c r="S10" s="11"/>
       <c r="T10" s="11"/>
-      <c r="U10" s="19">
+      <c r="U10" s="11"/>
+      <c r="V10" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" s="5" t="s">
         <v>33</v>
       </c>
@@ -1434,12 +1459,15 @@
       <c r="R11" s="13"/>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
-      <c r="U11" s="19">
+      <c r="U11" s="14">
+        <v>6</v>
+      </c>
+      <c r="V11" s="46">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="5" t="s">
         <v>34</v>
       </c>
@@ -1486,12 +1514,15 @@
         <v>4</v>
       </c>
       <c r="T12" s="11"/>
-      <c r="U12" s="19">
+      <c r="U12" s="11">
+        <v>12</v>
+      </c>
+      <c r="V12" s="19">
         <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="5" t="s">
         <v>45</v>
       </c>
@@ -1524,12 +1555,13 @@
         <v>4</v>
       </c>
       <c r="T13" s="14"/>
-      <c r="U13" s="19">
+      <c r="U13" s="14"/>
+      <c r="V13" s="19">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:22">
       <c r="A14" s="5" t="s">
         <v>35</v>
       </c>
@@ -1560,12 +1592,13 @@
       <c r="R14" s="3"/>
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
-      <c r="U14" s="19">
+      <c r="U14" s="11"/>
+      <c r="V14" s="46">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:22">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
@@ -1616,12 +1649,15 @@
         <v>2</v>
       </c>
       <c r="T15" s="14"/>
-      <c r="U15" s="19">
+      <c r="U15" s="14">
+        <v>3</v>
+      </c>
+      <c r="V15" s="19">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="5" t="s">
         <v>37</v>
       </c>
@@ -1648,12 +1684,13 @@
       <c r="R16" s="3"/>
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
-      <c r="U16" s="19">
+      <c r="U16" s="11"/>
+      <c r="V16" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:21">
+    <row r="17" spans="1:22">
       <c r="A17" s="5" t="s">
         <v>38</v>
       </c>
@@ -1682,12 +1719,13 @@
       <c r="R17" s="13"/>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
-      <c r="U17" s="19">
+      <c r="U17" s="14"/>
+      <c r="V17" s="19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:21">
+    <row r="18" spans="1:22">
       <c r="A18" s="5" t="s">
         <v>41</v>
       </c>
@@ -1740,12 +1778,15 @@
       <c r="T18" s="11">
         <v>2</v>
       </c>
-      <c r="U18" s="19">
+      <c r="U18" s="11">
+        <v>6</v>
+      </c>
+      <c r="V18" s="19">
         <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" thickBot="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>42</v>
       </c>
@@ -1782,27 +1823,28 @@
       <c r="R19" s="16"/>
       <c r="S19" s="18"/>
       <c r="T19" s="18"/>
-      <c r="U19" s="36">
+      <c r="U19" s="18"/>
+      <c r="V19" s="36">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:21">
+    <row r="20" spans="1:22">
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:22">
       <c r="N21" s="1"/>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:22">
       <c r="N22" s="1"/>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:22">
       <c r="N23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="Q1:T2"/>
+    <mergeCell ref="V1:V2"/>
+    <mergeCell ref="Q1:U2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="D1:D2"/>

</xml_diff>

<commit_message>
chg: Updated available ordnance and start time for D9.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
-    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
+    <sheet name="D9 -&gt;" sheetId="2" r:id="rId1"/>
+    <sheet name="D1-D8" sheetId="1" r:id="rId2"/>
     <sheet name="Ark3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
   <si>
     <t>D0</t>
   </si>
@@ -173,13 +173,67 @@
   </si>
   <si>
     <t>D8.2</t>
+  </si>
+  <si>
+    <t>D9.1</t>
+  </si>
+  <si>
+    <t>From D8</t>
+  </si>
+  <si>
+    <t>D9.2</t>
+  </si>
+  <si>
+    <t>D10.1</t>
+  </si>
+  <si>
+    <t>D10.2</t>
+  </si>
+  <si>
+    <t>D11.1</t>
+  </si>
+  <si>
+    <t>D11.2</t>
+  </si>
+  <si>
+    <t>D12.1</t>
+  </si>
+  <si>
+    <t>D12.2</t>
+  </si>
+  <si>
+    <t>D13.1</t>
+  </si>
+  <si>
+    <t>D13.2</t>
+  </si>
+  <si>
+    <t>D14.1</t>
+  </si>
+  <si>
+    <t>D14.2</t>
+  </si>
+  <si>
+    <t>D15.1</t>
+  </si>
+  <si>
+    <t>D15.2</t>
+  </si>
+  <si>
+    <t>D16.1</t>
+  </si>
+  <si>
+    <t>D16.2</t>
+  </si>
+  <si>
+    <t>D8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +276,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -518,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -611,6 +699,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,7 +726,118 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -660,6 +862,113 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>847724</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TekstSylinder 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="76200" y="4095750"/>
+          <a:ext cx="9372599" cy="1895475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nb-NO" sz="1400" b="1"/>
+            <a:t>NOTES:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>All other ordnance is unlimited.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Request for specific ordnance can be forwarded to CJTF HQ (Mission designer). Depending on the situation, expect between 1-6 events from ordnance is requested until it is available.</a:t>
+          </a:r>
+          <a:endParaRPr lang="nb-NO" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>304799</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
@@ -675,7 +984,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1050,7 +1359,722 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+      <selection activeCell="H31" sqref="H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4" customWidth="1"/>
+    <col min="8" max="9" width="5.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" customWidth="1"/>
+    <col min="14" max="14" width="5.28515625" customWidth="1"/>
+    <col min="15" max="15" width="5.140625" customWidth="1"/>
+    <col min="16" max="16" width="5.28515625" customWidth="1"/>
+    <col min="17" max="17" width="5" customWidth="1"/>
+    <col min="18" max="18" width="4.85546875" customWidth="1"/>
+    <col min="19" max="19" width="5.140625" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="49" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="52" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="39.75" customHeight="1">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="56"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="57"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A3" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="63" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="L3" s="63" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="N3" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="O3" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q3" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="T3" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="U3" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="V3" s="64" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="67">
+        <v>47</v>
+      </c>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="70"/>
+      <c r="T4" s="70"/>
+      <c r="U4" s="70"/>
+      <c r="V4" s="71">
+        <f t="shared" ref="V4:V19" si="0">SUM(C4:E4)-SUM(F4:U4)</f>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" s="65" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="72">
+        <v>10</v>
+      </c>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+      <c r="L5" s="74"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
+      <c r="Q5" s="74"/>
+      <c r="R5" s="74"/>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+      <c r="U5" s="75"/>
+      <c r="V5" s="71">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="76">
+        <v>6</v>
+      </c>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="70"/>
+      <c r="T6" s="70"/>
+      <c r="U6" s="70"/>
+      <c r="V6" s="71">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="65" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="72">
+        <v>9</v>
+      </c>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="75"/>
+      <c r="T7" s="75"/>
+      <c r="U7" s="75"/>
+      <c r="V7" s="71">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="65" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="76">
+        <v>6</v>
+      </c>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="77"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+      <c r="R8" s="69"/>
+      <c r="S8" s="70"/>
+      <c r="T8" s="70"/>
+      <c r="U8" s="70"/>
+      <c r="V8" s="71">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="65" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="72">
+        <v>6</v>
+      </c>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="78"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+      <c r="U9" s="75"/>
+      <c r="V9" s="71">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="76">
+        <v>20</v>
+      </c>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="68">
+        <v>8</v>
+      </c>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="77"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
+      <c r="S10" s="70"/>
+      <c r="T10" s="70"/>
+      <c r="U10" s="70"/>
+      <c r="V10" s="71">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="72">
+        <v>3</v>
+      </c>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="74"/>
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="74"/>
+      <c r="L11" s="74"/>
+      <c r="M11" s="74"/>
+      <c r="N11" s="74"/>
+      <c r="O11" s="74"/>
+      <c r="P11" s="74"/>
+      <c r="Q11" s="74"/>
+      <c r="R11" s="74"/>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+      <c r="U11" s="75"/>
+      <c r="V11" s="79">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="65" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="76">
+        <v>40</v>
+      </c>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="68">
+        <v>10</v>
+      </c>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="69"/>
+      <c r="R12" s="69"/>
+      <c r="S12" s="70"/>
+      <c r="T12" s="70"/>
+      <c r="U12" s="70"/>
+      <c r="V12" s="71">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="72">
+        <v>5</v>
+      </c>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="74"/>
+      <c r="L13" s="74"/>
+      <c r="M13" s="74"/>
+      <c r="N13" s="78"/>
+      <c r="O13" s="74"/>
+      <c r="P13" s="74"/>
+      <c r="Q13" s="74"/>
+      <c r="R13" s="74"/>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+      <c r="U13" s="75"/>
+      <c r="V13" s="71">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="76">
+        <v>3</v>
+      </c>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="77"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="69"/>
+      <c r="R14" s="69"/>
+      <c r="S14" s="70"/>
+      <c r="T14" s="70"/>
+      <c r="U14" s="70"/>
+      <c r="V14" s="79">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="72">
+        <v>47</v>
+      </c>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73">
+        <v>1</v>
+      </c>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
+      <c r="K15" s="74"/>
+      <c r="L15" s="74"/>
+      <c r="M15" s="74"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="74"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="74"/>
+      <c r="R15" s="74"/>
+      <c r="S15" s="75"/>
+      <c r="T15" s="75"/>
+      <c r="U15" s="75"/>
+      <c r="V15" s="71">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="76">
+        <v>0</v>
+      </c>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+      <c r="R16" s="69"/>
+      <c r="S16" s="70"/>
+      <c r="T16" s="70"/>
+      <c r="U16" s="70"/>
+      <c r="V16" s="79">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="72">
+        <v>10</v>
+      </c>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="74"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="74"/>
+      <c r="J17" s="74"/>
+      <c r="K17" s="74"/>
+      <c r="L17" s="74"/>
+      <c r="M17" s="74"/>
+      <c r="N17" s="78"/>
+      <c r="O17" s="74"/>
+      <c r="P17" s="74"/>
+      <c r="Q17" s="74"/>
+      <c r="R17" s="74"/>
+      <c r="S17" s="75"/>
+      <c r="T17" s="75"/>
+      <c r="U17" s="75"/>
+      <c r="V17" s="71">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" s="65" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="66" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="80">
+        <v>42</v>
+      </c>
+      <c r="D18" s="80"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="82">
+        <v>8</v>
+      </c>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+      <c r="R18" s="69"/>
+      <c r="S18" s="70"/>
+      <c r="T18" s="70"/>
+      <c r="U18" s="70"/>
+      <c r="V18" s="71">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A19" s="83" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="85">
+        <v>60</v>
+      </c>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="87"/>
+      <c r="I19" s="87"/>
+      <c r="J19" s="87"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="88"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="87"/>
+      <c r="R19" s="87"/>
+      <c r="S19" s="89"/>
+      <c r="T19" s="89"/>
+      <c r="U19" s="89"/>
+      <c r="V19" s="90">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:22">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="N23" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="Q1:U2"/>
+    <mergeCell ref="V1:V2"/>
+  </mergeCells>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:V23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1072,13 +2096,13 @@
     <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="45" t="s">
         <v>44</v>
       </c>
       <c r="F1" s="8"/>
@@ -1092,23 +2116,23 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="40" t="s">
+      <c r="Q1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="40"/>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="38" t="s">
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="69.75" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="34"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -1120,12 +2144,12 @@
       <c r="N2" s="34"/>
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="39"/>
+      <c r="Q2" s="42"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="42"/>
+      <c r="T2" s="42"/>
+      <c r="U2" s="42"/>
+      <c r="V2" s="40"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1">
       <c r="A3" s="10" t="s">
@@ -1462,7 +2486,7 @@
       <c r="U11" s="14">
         <v>6</v>
       </c>
-      <c r="V11" s="46">
+      <c r="V11" s="38">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1593,7 +2617,7 @@
       <c r="S14" s="11"/>
       <c r="T14" s="11"/>
       <c r="U14" s="11"/>
-      <c r="V14" s="46">
+      <c r="V14" s="38">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -1685,7 +2709,7 @@
       <c r="S16" s="11"/>
       <c r="T16" s="11"/>
       <c r="U16" s="11"/>
-      <c r="V16" s="46">
+      <c r="V16" s="38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1855,19 +2879,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>

</xml_diff>

<commit_message>
chg: Updates for D10
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -702,55 +702,10 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,6 +794,51 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -877,7 +877,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -984,7 +984,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1386,659 +1386,665 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="49" t="s">
+      <c r="A1" s="39"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="51" t="s">
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="N1" s="40"/>
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="52" t="s">
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="39.75" customHeight="1">
+      <c r="A2" s="41"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
+      <c r="Q2" s="80"/>
+      <c r="R2" s="80"/>
+      <c r="S2" s="80"/>
+      <c r="T2" s="80"/>
+      <c r="U2" s="80"/>
+      <c r="V2" s="82"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A3" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="57"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A3" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="62" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="63" t="s">
+      <c r="G3" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="63" t="s">
+      <c r="J3" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="63" t="s">
+      <c r="K3" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="63" t="s">
+      <c r="L3" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="63" t="s">
+      <c r="M3" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="63" t="s">
+      <c r="N3" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="63" t="s">
+      <c r="O3" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="63" t="s">
+      <c r="P3" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="63" t="s">
+      <c r="Q3" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="63" t="s">
+      <c r="R3" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="63" t="s">
+      <c r="S3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="T3" s="63" t="s">
+      <c r="T3" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="63" t="s">
+      <c r="U3" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="V3" s="64" t="s">
+      <c r="V3" s="49" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="66" t="s">
+      <c r="B4" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="67">
+      <c r="C4" s="52">
         <v>47</v>
       </c>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="70"/>
-      <c r="T4" s="70"/>
-      <c r="U4" s="70"/>
-      <c r="V4" s="71">
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+      <c r="L4" s="54"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="54"/>
+      <c r="O4" s="54"/>
+      <c r="P4" s="54"/>
+      <c r="Q4" s="54"/>
+      <c r="R4" s="54"/>
+      <c r="S4" s="55"/>
+      <c r="T4" s="55"/>
+      <c r="U4" s="55"/>
+      <c r="V4" s="56">
         <f t="shared" ref="V4:V19" si="0">SUM(C4:E4)-SUM(F4:U4)</f>
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="72">
+      <c r="C5" s="57">
         <v>10</v>
       </c>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-      <c r="I5" s="74"/>
-      <c r="J5" s="74"/>
-      <c r="K5" s="74"/>
-      <c r="L5" s="74"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="74"/>
-      <c r="S5" s="75"/>
-      <c r="T5" s="75"/>
-      <c r="U5" s="75"/>
-      <c r="V5" s="71">
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="60"/>
+      <c r="T5" s="60"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="56">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="61">
         <v>6</v>
       </c>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="69"/>
-      <c r="S6" s="70"/>
-      <c r="T6" s="70"/>
-      <c r="U6" s="70"/>
-      <c r="V6" s="71">
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="54"/>
+      <c r="S6" s="55"/>
+      <c r="T6" s="55"/>
+      <c r="U6" s="55"/>
+      <c r="V6" s="56">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:22">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="72">
+      <c r="C7" s="57">
         <v>9</v>
       </c>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="74"/>
-      <c r="K7" s="74"/>
-      <c r="L7" s="74"/>
-      <c r="M7" s="74"/>
-      <c r="N7" s="74"/>
-      <c r="O7" s="74"/>
-      <c r="P7" s="74"/>
-      <c r="Q7" s="74"/>
-      <c r="R7" s="74"/>
-      <c r="S7" s="75"/>
-      <c r="T7" s="75"/>
-      <c r="U7" s="75"/>
-      <c r="V7" s="71">
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="60"/>
+      <c r="U7" s="60"/>
+      <c r="V7" s="56">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:22">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="66" t="s">
+      <c r="B8" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="76">
+      <c r="C8" s="61">
         <v>6</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="77"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-      <c r="R8" s="69"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="71">
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="54"/>
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="54"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="54"/>
+      <c r="S8" s="55"/>
+      <c r="T8" s="55"/>
+      <c r="U8" s="55"/>
+      <c r="V8" s="56">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:22">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="66" t="s">
+      <c r="B9" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="72">
+      <c r="C9" s="57">
         <v>6</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="74"/>
-      <c r="H9" s="74"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="74"/>
-      <c r="K9" s="74"/>
-      <c r="L9" s="74"/>
-      <c r="M9" s="74"/>
-      <c r="N9" s="78"/>
-      <c r="O9" s="74"/>
-      <c r="P9" s="74"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="74"/>
-      <c r="S9" s="75"/>
-      <c r="T9" s="75"/>
-      <c r="U9" s="75"/>
-      <c r="V9" s="71">
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="59"/>
+      <c r="N9" s="63"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="59"/>
+      <c r="Q9" s="59"/>
+      <c r="R9" s="59"/>
+      <c r="S9" s="60"/>
+      <c r="T9" s="60"/>
+      <c r="U9" s="60"/>
+      <c r="V9" s="56">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:22">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="76">
+      <c r="C10" s="61">
         <v>20</v>
       </c>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="68">
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="53">
         <v>8</v>
       </c>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="77"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-      <c r="R10" s="69"/>
-      <c r="S10" s="70"/>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
-      <c r="V10" s="71">
+      <c r="G10" s="54"/>
+      <c r="H10" s="54"/>
+      <c r="I10" s="54"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="54"/>
+      <c r="M10" s="54"/>
+      <c r="N10" s="62"/>
+      <c r="O10" s="54"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="55"/>
+      <c r="T10" s="55"/>
+      <c r="U10" s="55"/>
+      <c r="V10" s="56">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:22">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="72">
+      <c r="C11" s="57">
         <v>3</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="73"/>
-      <c r="G11" s="74"/>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="74"/>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-      <c r="O11" s="74"/>
-      <c r="P11" s="74"/>
-      <c r="Q11" s="74"/>
-      <c r="R11" s="74"/>
-      <c r="S11" s="75"/>
-      <c r="T11" s="75"/>
-      <c r="U11" s="75"/>
-      <c r="V11" s="79">
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="59"/>
+      <c r="Q11" s="59"/>
+      <c r="R11" s="59"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="60"/>
+      <c r="V11" s="64">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:22">
-      <c r="A12" s="65" t="s">
+      <c r="A12" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="66" t="s">
+      <c r="B12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="76">
+      <c r="C12" s="61">
         <v>40</v>
       </c>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="68">
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="53">
         <v>10</v>
       </c>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="69"/>
-      <c r="S12" s="70"/>
-      <c r="T12" s="70"/>
-      <c r="U12" s="70"/>
-      <c r="V12" s="71">
+      <c r="G12" s="54"/>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="54"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="54"/>
+      <c r="P12" s="54"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="55"/>
+      <c r="T12" s="55"/>
+      <c r="U12" s="55"/>
+      <c r="V12" s="56">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:22">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="66" t="s">
+      <c r="B13" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="72">
+      <c r="C13" s="57">
         <v>5</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="74"/>
-      <c r="I13" s="74"/>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
-      <c r="M13" s="74"/>
-      <c r="N13" s="78"/>
-      <c r="O13" s="74"/>
-      <c r="P13" s="74"/>
-      <c r="Q13" s="74"/>
-      <c r="R13" s="74"/>
-      <c r="S13" s="75"/>
-      <c r="T13" s="75"/>
-      <c r="U13" s="75"/>
-      <c r="V13" s="71">
-        <f t="shared" si="0"/>
-        <v>5</v>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59">
+        <v>2</v>
+      </c>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="59"/>
+      <c r="Q13" s="59"/>
+      <c r="R13" s="59"/>
+      <c r="S13" s="60"/>
+      <c r="T13" s="60"/>
+      <c r="U13" s="60"/>
+      <c r="V13" s="64">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:22">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="76">
+      <c r="C14" s="61">
         <v>3</v>
       </c>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="77"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="69"/>
-      <c r="R14" s="69"/>
-      <c r="S14" s="70"/>
-      <c r="T14" s="70"/>
-      <c r="U14" s="70"/>
-      <c r="V14" s="79">
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="54"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="62"/>
+      <c r="O14" s="54"/>
+      <c r="P14" s="54"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="54"/>
+      <c r="S14" s="55"/>
+      <c r="T14" s="55"/>
+      <c r="U14" s="55"/>
+      <c r="V14" s="64">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:22">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="72">
+      <c r="C15" s="57">
         <v>47</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="72"/>
-      <c r="F15" s="73">
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58">
         <v>1</v>
       </c>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="74"/>
-      <c r="N15" s="74"/>
-      <c r="O15" s="74"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="74"/>
-      <c r="R15" s="74"/>
-      <c r="S15" s="75"/>
-      <c r="T15" s="75"/>
-      <c r="U15" s="75"/>
-      <c r="V15" s="71">
-        <f t="shared" si="0"/>
-        <v>46</v>
+      <c r="G15" s="59">
+        <v>4</v>
+      </c>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="59"/>
+      <c r="P15" s="59"/>
+      <c r="Q15" s="59"/>
+      <c r="R15" s="59"/>
+      <c r="S15" s="60"/>
+      <c r="T15" s="60"/>
+      <c r="U15" s="60"/>
+      <c r="V15" s="56">
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="66" t="s">
+      <c r="B16" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="76">
+      <c r="C16" s="61">
         <v>0</v>
       </c>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="77"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-      <c r="Q16" s="69"/>
-      <c r="R16" s="69"/>
-      <c r="S16" s="70"/>
-      <c r="T16" s="70"/>
-      <c r="U16" s="70"/>
-      <c r="V16" s="79">
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="54"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
+      <c r="K16" s="54"/>
+      <c r="L16" s="54"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="54"/>
+      <c r="P16" s="54"/>
+      <c r="Q16" s="54"/>
+      <c r="R16" s="54"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="66" t="s">
+      <c r="B17" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="72">
+      <c r="C17" s="57">
         <v>10</v>
       </c>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="74"/>
-      <c r="H17" s="74"/>
-      <c r="I17" s="74"/>
-      <c r="J17" s="74"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="74"/>
-      <c r="N17" s="78"/>
-      <c r="O17" s="74"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="74"/>
-      <c r="R17" s="74"/>
-      <c r="S17" s="75"/>
-      <c r="T17" s="75"/>
-      <c r="U17" s="75"/>
-      <c r="V17" s="71">
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="59"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="59"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="59"/>
+      <c r="P17" s="59"/>
+      <c r="Q17" s="59"/>
+      <c r="R17" s="59"/>
+      <c r="S17" s="60"/>
+      <c r="T17" s="60"/>
+      <c r="U17" s="60"/>
+      <c r="V17" s="56">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="80">
+      <c r="C18" s="65">
         <v>42</v>
       </c>
-      <c r="D18" s="80"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="82">
+      <c r="D18" s="65"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="67">
         <v>8</v>
       </c>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="70"/>
-      <c r="V18" s="71">
-        <f t="shared" si="0"/>
-        <v>34</v>
+      <c r="G18" s="54">
+        <v>11</v>
+      </c>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="54"/>
+      <c r="L18" s="54"/>
+      <c r="M18" s="54"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="54"/>
+      <c r="P18" s="54"/>
+      <c r="Q18" s="54"/>
+      <c r="R18" s="54"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="56">
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A19" s="83" t="s">
+      <c r="A19" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="85">
+      <c r="C19" s="70">
         <v>60</v>
       </c>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="87"/>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="88"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="87"/>
-      <c r="Q19" s="87"/>
-      <c r="R19" s="87"/>
-      <c r="S19" s="89"/>
-      <c r="T19" s="89"/>
-      <c r="U19" s="89"/>
-      <c r="V19" s="90">
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="72"/>
+      <c r="H19" s="72"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="73"/>
+      <c r="O19" s="72"/>
+      <c r="P19" s="72"/>
+      <c r="Q19" s="72"/>
+      <c r="R19" s="72"/>
+      <c r="S19" s="74"/>
+      <c r="T19" s="74"/>
+      <c r="U19" s="74"/>
+      <c r="V19" s="75">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -2096,13 +2102,13 @@
     <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="89" t="s">
         <v>44</v>
       </c>
       <c r="F1" s="8"/>
@@ -2116,23 +2122,23 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="39" t="s">
+      <c r="R1" s="85"/>
+      <c r="S1" s="85"/>
+      <c r="T1" s="85"/>
+      <c r="U1" s="85"/>
+      <c r="V1" s="83" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="69.75" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="34"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="45"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="89"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -2144,12 +2150,12 @@
       <c r="N2" s="34"/>
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="40"/>
+      <c r="Q2" s="86"/>
+      <c r="R2" s="86"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="84"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1">
       <c r="A3" s="10" t="s">

</xml_diff>

<commit_message>
chg: Updated ordnance after D10.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -877,7 +877,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -984,7 +984,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1416,7 +1416,7 @@
       <c r="T1" s="79"/>
       <c r="U1" s="79"/>
       <c r="V1" s="81" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="39.75" customHeight="1">
@@ -1721,7 +1721,9 @@
         <v>8</v>
       </c>
       <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
+      <c r="H10" s="54">
+        <v>8</v>
+      </c>
       <c r="I10" s="54"/>
       <c r="J10" s="54"/>
       <c r="K10" s="54"/>
@@ -1737,7 +1739,7 @@
       <c r="U10" s="55"/>
       <c r="V10" s="56">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1789,7 +1791,9 @@
         <v>10</v>
       </c>
       <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
+      <c r="H12" s="54">
+        <v>2</v>
+      </c>
       <c r="I12" s="54"/>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
@@ -1805,7 +1809,7 @@
       <c r="U12" s="55"/>
       <c r="V12" s="56">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1894,7 +1898,9 @@
       <c r="G15" s="59">
         <v>4</v>
       </c>
-      <c r="H15" s="59"/>
+      <c r="H15" s="59">
+        <v>2</v>
+      </c>
       <c r="I15" s="59"/>
       <c r="J15" s="59"/>
       <c r="K15" s="59"/>
@@ -1910,7 +1916,7 @@
       <c r="U15" s="60"/>
       <c r="V15" s="56">
         <f t="shared" si="0"/>
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:22">

</xml_diff>

<commit_message>
chg: Added VID intsum from D10, updated ordnance, updated time and weather for D11.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -877,7 +877,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -984,7 +984,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1416,7 +1416,7 @@
       <c r="T1" s="79"/>
       <c r="U1" s="79"/>
       <c r="V1" s="81" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="39.75" customHeight="1">
@@ -1794,7 +1794,9 @@
       <c r="H12" s="54">
         <v>2</v>
       </c>
-      <c r="I12" s="54"/>
+      <c r="I12" s="54">
+        <v>11</v>
+      </c>
       <c r="J12" s="54"/>
       <c r="K12" s="54"/>
       <c r="L12" s="54"/>
@@ -1809,7 +1811,7 @@
       <c r="U12" s="55"/>
       <c r="V12" s="56">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1901,7 +1903,9 @@
       <c r="H15" s="59">
         <v>2</v>
       </c>
-      <c r="I15" s="59"/>
+      <c r="I15" s="59">
+        <v>1</v>
+      </c>
       <c r="J15" s="59"/>
       <c r="K15" s="59"/>
       <c r="L15" s="59"/>
@@ -1916,7 +1920,7 @@
       <c r="U15" s="60"/>
       <c r="V15" s="56">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -2004,7 +2008,9 @@
         <v>11</v>
       </c>
       <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
+      <c r="I18" s="54">
+        <v>3</v>
+      </c>
       <c r="J18" s="54"/>
       <c r="K18" s="54"/>
       <c r="L18" s="54"/>
@@ -2019,7 +2025,7 @@
       <c r="U18" s="55"/>
       <c r="V18" s="56">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
chg: Updated weather, time of day and ordnance for D11.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -877,7 +877,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -984,7 +984,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1359,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1416,7 +1416,7 @@
       <c r="T1" s="79"/>
       <c r="U1" s="79"/>
       <c r="V1" s="81" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="39.75" customHeight="1">
@@ -1655,7 +1655,9 @@
       <c r="G8" s="54"/>
       <c r="H8" s="54"/>
       <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
+      <c r="J8" s="54">
+        <v>2</v>
+      </c>
       <c r="K8" s="54"/>
       <c r="L8" s="54"/>
       <c r="M8" s="54"/>
@@ -1667,9 +1669,9 @@
       <c r="S8" s="55"/>
       <c r="T8" s="55"/>
       <c r="U8" s="55"/>
-      <c r="V8" s="56">
+      <c r="V8" s="64">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1688,7 +1690,9 @@
       <c r="G9" s="59"/>
       <c r="H9" s="59"/>
       <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
+      <c r="J9" s="59">
+        <v>4</v>
+      </c>
       <c r="K9" s="59"/>
       <c r="L9" s="59"/>
       <c r="M9" s="59"/>
@@ -1700,9 +1704,9 @@
       <c r="S9" s="60"/>
       <c r="T9" s="60"/>
       <c r="U9" s="60"/>
-      <c r="V9" s="56">
+      <c r="V9" s="64">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1737,7 +1741,7 @@
       <c r="S10" s="55"/>
       <c r="T10" s="55"/>
       <c r="U10" s="55"/>
-      <c r="V10" s="56">
+      <c r="V10" s="64">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
@@ -1797,7 +1801,9 @@
       <c r="I12" s="54">
         <v>11</v>
       </c>
-      <c r="J12" s="54"/>
+      <c r="J12" s="54">
+        <v>3</v>
+      </c>
       <c r="K12" s="54"/>
       <c r="L12" s="54"/>
       <c r="M12" s="54"/>
@@ -1811,7 +1817,7 @@
       <c r="U12" s="55"/>
       <c r="V12" s="56">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1906,7 +1912,9 @@
       <c r="I15" s="59">
         <v>1</v>
       </c>
-      <c r="J15" s="59"/>
+      <c r="J15" s="59">
+        <v>9</v>
+      </c>
       <c r="K15" s="59"/>
       <c r="L15" s="59"/>
       <c r="M15" s="59"/>
@@ -1920,7 +1928,7 @@
       <c r="U15" s="60"/>
       <c r="V15" s="56">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -2011,7 +2019,9 @@
       <c r="I18" s="54">
         <v>3</v>
       </c>
-      <c r="J18" s="54"/>
+      <c r="J18" s="54">
+        <v>9</v>
+      </c>
       <c r="K18" s="54"/>
       <c r="L18" s="54"/>
       <c r="M18" s="54"/>
@@ -2025,7 +2035,7 @@
       <c r="U18" s="55"/>
       <c r="V18" s="56">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
chg: Updated time and weather for D12.1. Added VID intusm from D11. Added JFC direction and guidance for D12
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAR Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAR Ordnance.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <t>D0</t>
   </si>
@@ -227,6 +227,12 @@
   </si>
   <si>
     <t>D8</t>
+  </si>
+  <si>
+    <t>ADDED D12</t>
+  </si>
+  <si>
+    <t>Ordnance Airbases</t>
   </si>
 </sst>
 </file>
@@ -304,8 +310,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -337,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -602,11 +609,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="5"/>
@@ -702,9 +729,7 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -765,9 +790,6 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,6 +861,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -877,7 +914,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -948,6 +985,40 @@
             </a:rPr>
             <a:t>Request for specific ordnance can be forwarded to CJTF HQ (Mission designer). Depending on the situation, expect between 1-6 events from ordnance is requested until it is available.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Note on D12: ordnance was split</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> into ordnance for airbases and ordnance for CVN.</a:t>
+          </a:r>
           <a:endParaRPr lang="nb-NO" sz="1100">
             <a:solidFill>
               <a:schemeClr val="dk1"/>
@@ -984,7 +1055,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1359,7 +1430,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1386,689 +1457,755 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
-      <c r="A1" s="39"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="76" t="s">
+      <c r="A1" s="89" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="90"/>
+      <c r="C1" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="78" t="s">
+      <c r="D1" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="78" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="40"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="79" t="s">
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="79"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="81" t="s">
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="78" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="39.75" customHeight="1">
+      <c r="A2" s="91"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="74"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="77"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="77"/>
+      <c r="T2" s="77"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="79"/>
+    </row>
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A3" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="K3" s="46" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="39.75" customHeight="1">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="80"/>
-      <c r="R2" s="80"/>
-      <c r="S2" s="80"/>
-      <c r="T2" s="80"/>
-      <c r="U2" s="80"/>
-      <c r="V2" s="82"/>
-    </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A3" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="47" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="48" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>51</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="L3" s="48" t="s">
+      <c r="L3" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="48" t="s">
+      <c r="M3" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="48" t="s">
+      <c r="N3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="O3" s="48" t="s">
+      <c r="O3" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="P3" s="48" t="s">
+      <c r="P3" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="48" t="s">
+      <c r="Q3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="R3" s="48" t="s">
+      <c r="R3" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="48" t="s">
+      <c r="S3" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="T3" s="48" t="s">
+      <c r="T3" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="U3" s="48" t="s">
+      <c r="U3" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="V3" s="47" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="50">
         <v>47</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="54"/>
-      <c r="O4" s="54"/>
-      <c r="P4" s="54"/>
-      <c r="Q4" s="54"/>
-      <c r="R4" s="54"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
-      <c r="V4" s="56">
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52">
+        <v>47</v>
+      </c>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="53"/>
+      <c r="T4" s="53"/>
+      <c r="U4" s="53"/>
+      <c r="V4" s="54">
         <f t="shared" ref="V4:V19" si="0">SUM(C4:E4)-SUM(F4:U4)</f>
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:22">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="57">
+      <c r="C5" s="55">
         <v>10</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59"/>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
-      <c r="V5" s="56">
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57">
+        <v>10</v>
+      </c>
+      <c r="M5" s="57"/>
+      <c r="N5" s="57"/>
+      <c r="O5" s="57"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
+      <c r="R5" s="57"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="58"/>
+      <c r="V5" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="59">
+        <v>6</v>
+      </c>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
+      <c r="L6" s="52">
+        <v>6</v>
+      </c>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="52"/>
+      <c r="P6" s="52"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="52"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="53"/>
+      <c r="U6" s="53"/>
+      <c r="V6" s="54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="55">
+        <v>9</v>
+      </c>
+      <c r="D7" s="55">
+        <v>5</v>
+      </c>
+      <c r="E7" s="55"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="57">
+        <v>8</v>
+      </c>
+      <c r="M7" s="57"/>
+      <c r="N7" s="57"/>
+      <c r="O7" s="57"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
+      <c r="R7" s="57"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="58"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="54">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="59">
+        <v>6</v>
+      </c>
+      <c r="D8" s="59">
+        <v>10</v>
+      </c>
+      <c r="E8" s="59"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="52">
+        <v>2</v>
+      </c>
+      <c r="K8" s="52"/>
+      <c r="L8" s="52">
+        <v>14</v>
+      </c>
+      <c r="M8" s="52"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="52"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="55">
+        <v>6</v>
+      </c>
+      <c r="D9" s="55">
+        <v>20</v>
+      </c>
+      <c r="E9" s="55"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57">
+        <v>4</v>
+      </c>
+      <c r="K9" s="57"/>
+      <c r="L9" s="57">
+        <v>12</v>
+      </c>
+      <c r="M9" s="57"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
+      <c r="R9" s="57"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="58"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="88">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" s="51" t="s">
+    <row r="10" spans="1:22">
+      <c r="A10" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="59">
+        <v>20</v>
+      </c>
+      <c r="D10" s="59">
+        <v>10</v>
+      </c>
+      <c r="E10" s="59"/>
+      <c r="F10" s="51">
+        <v>8</v>
+      </c>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52">
+        <v>8</v>
+      </c>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52">
+        <v>7</v>
+      </c>
+      <c r="M10" s="52"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="52"/>
+      <c r="S10" s="53"/>
+      <c r="T10" s="53"/>
+      <c r="U10" s="53"/>
+      <c r="V10" s="88">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="61">
-        <v>6</v>
-      </c>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="54"/>
-      <c r="N6" s="54"/>
-      <c r="O6" s="54"/>
-      <c r="P6" s="54"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="54"/>
-      <c r="S6" s="55"/>
-      <c r="T6" s="55"/>
-      <c r="U6" s="55"/>
-      <c r="V6" s="56">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="50" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="57">
-        <v>9</v>
-      </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
-      <c r="V7" s="56">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8" s="50" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="61">
-        <v>6</v>
-      </c>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54">
+      <c r="C11" s="55">
+        <v>3</v>
+      </c>
+      <c r="D11" s="55">
+        <v>15</v>
+      </c>
+      <c r="E11" s="55"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57">
         <v>2</v>
       </c>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="54"/>
-      <c r="S8" s="55"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="55"/>
-      <c r="V8" s="64">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="57">
-        <v>6</v>
-      </c>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59">
-        <v>4</v>
-      </c>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="63"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="60"/>
-      <c r="U9" s="60"/>
-      <c r="V9" s="64">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="61">
-        <v>20</v>
-      </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="53">
-        <v>8</v>
-      </c>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54">
-        <v>8</v>
-      </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
-      <c r="M10" s="54"/>
-      <c r="N10" s="62"/>
-      <c r="O10" s="54"/>
-      <c r="P10" s="54"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="54"/>
-      <c r="S10" s="55"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="55"/>
-      <c r="V10" s="64">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22">
-      <c r="A11" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="57">
-        <v>3</v>
-      </c>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="59"/>
-      <c r="L11" s="59"/>
-      <c r="M11" s="59"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="59"/>
-      <c r="Q11" s="59"/>
-      <c r="R11" s="59"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="60"/>
-      <c r="U11" s="60"/>
-      <c r="V11" s="64">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22">
-      <c r="A12" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="51" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="61">
-        <v>40</v>
-      </c>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="53">
-        <v>10</v>
-      </c>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54">
-        <v>2</v>
-      </c>
-      <c r="I12" s="54">
-        <v>11</v>
-      </c>
-      <c r="J12" s="54">
-        <v>3</v>
-      </c>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
-      <c r="M12" s="54"/>
-      <c r="N12" s="62"/>
-      <c r="O12" s="54"/>
-      <c r="P12" s="54"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="54"/>
-      <c r="S12" s="55"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="55"/>
-      <c r="V12" s="56">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="57">
-        <v>5</v>
-      </c>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="59">
-        <v>2</v>
-      </c>
-      <c r="H13" s="59"/>
-      <c r="I13" s="59"/>
-      <c r="J13" s="59"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="59"/>
-      <c r="M13" s="59"/>
-      <c r="N13" s="63"/>
-      <c r="O13" s="59"/>
-      <c r="P13" s="59"/>
-      <c r="Q13" s="59"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="60"/>
-      <c r="U13" s="60"/>
-      <c r="V13" s="64">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22">
-      <c r="A14" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="61">
-        <v>3</v>
-      </c>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="62"/>
-      <c r="O14" s="54"/>
-      <c r="P14" s="54"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="54"/>
-      <c r="S14" s="55"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="55"/>
-      <c r="V14" s="64">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22">
-      <c r="A15" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="57">
-        <v>47</v>
-      </c>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58">
-        <v>1</v>
-      </c>
-      <c r="G15" s="59">
-        <v>4</v>
-      </c>
-      <c r="H15" s="59">
-        <v>2</v>
-      </c>
-      <c r="I15" s="59">
-        <v>1</v>
-      </c>
-      <c r="J15" s="59">
-        <v>9</v>
-      </c>
-      <c r="K15" s="59"/>
-      <c r="L15" s="59"/>
-      <c r="M15" s="59"/>
-      <c r="N15" s="59"/>
-      <c r="O15" s="59"/>
-      <c r="P15" s="59"/>
-      <c r="Q15" s="59"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="60"/>
-      <c r="U15" s="60"/>
-      <c r="V15" s="56">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="50" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="61">
-        <v>0</v>
-      </c>
-      <c r="D16" s="61"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
-      <c r="M16" s="54"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="54"/>
-      <c r="P16" s="54"/>
-      <c r="Q16" s="54"/>
-      <c r="R16" s="54"/>
-      <c r="S16" s="55"/>
-      <c r="T16" s="55"/>
-      <c r="U16" s="55"/>
-      <c r="V16" s="64">
+      <c r="L11" s="57">
+        <v>16</v>
+      </c>
+      <c r="M11" s="57"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="58"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="88">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
+    <row r="12" spans="1:22">
+      <c r="A12" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="59">
+        <v>40</v>
+      </c>
+      <c r="D12" s="59">
+        <v>60</v>
+      </c>
+      <c r="E12" s="59"/>
+      <c r="F12" s="51">
+        <v>10</v>
+      </c>
+      <c r="G12" s="52"/>
+      <c r="H12" s="52">
+        <v>2</v>
+      </c>
+      <c r="I12" s="52">
+        <v>11</v>
+      </c>
+      <c r="J12" s="52">
+        <v>3</v>
+      </c>
+      <c r="K12" s="52">
+        <v>9</v>
+      </c>
+      <c r="L12" s="52">
+        <v>32</v>
+      </c>
+      <c r="M12" s="52"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="52"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="53"/>
+      <c r="U12" s="53"/>
+      <c r="V12" s="88">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="55">
+        <v>5</v>
+      </c>
+      <c r="D13" s="55">
+        <v>20</v>
+      </c>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="57">
+        <v>2</v>
+      </c>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="57"/>
+      <c r="P13" s="57"/>
+      <c r="Q13" s="57"/>
+      <c r="R13" s="57"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="58"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="88">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="59">
+        <v>3</v>
+      </c>
+      <c r="D14" s="59">
+        <v>30</v>
+      </c>
+      <c r="E14" s="59"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52">
+        <v>16</v>
+      </c>
+      <c r="M14" s="52"/>
+      <c r="N14" s="60"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="52"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="88">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="55">
+        <v>47</v>
+      </c>
+      <c r="D15" s="55">
+        <v>50</v>
+      </c>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56">
+        <v>1</v>
+      </c>
+      <c r="G15" s="57">
+        <v>4</v>
+      </c>
+      <c r="H15" s="57">
+        <v>2</v>
+      </c>
+      <c r="I15" s="57">
+        <v>1</v>
+      </c>
+      <c r="J15" s="57">
+        <v>9</v>
+      </c>
+      <c r="K15" s="57">
+        <v>4</v>
+      </c>
+      <c r="L15" s="57">
+        <v>30</v>
+      </c>
+      <c r="M15" s="57"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
+      <c r="R15" s="57"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="58"/>
+      <c r="U15" s="58"/>
+      <c r="V15" s="88">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="59">
+        <v>0</v>
+      </c>
+      <c r="D16" s="59">
+        <v>20</v>
+      </c>
+      <c r="E16" s="59"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52">
+        <v>20</v>
+      </c>
+      <c r="M16" s="52"/>
+      <c r="N16" s="60"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" spans="1:22">
-      <c r="A17" s="50" t="s">
+      <c r="A17" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="55">
         <v>10</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="59"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="59"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="59"/>
-      <c r="M17" s="59"/>
-      <c r="N17" s="63"/>
-      <c r="O17" s="59"/>
-      <c r="P17" s="59"/>
-      <c r="Q17" s="59"/>
-      <c r="R17" s="59"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="60"/>
-      <c r="U17" s="60"/>
-      <c r="V17" s="56">
+      <c r="D17" s="55">
+        <v>20</v>
+      </c>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="57">
+        <v>15</v>
+      </c>
+      <c r="M17" s="57"/>
+      <c r="N17" s="61"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
+      <c r="R17" s="57"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="58"/>
+      <c r="U17" s="58"/>
+      <c r="V17" s="88">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:22">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="51" t="s">
+      <c r="B18" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="65">
+      <c r="C18" s="62">
         <v>42</v>
       </c>
-      <c r="D18" s="65"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="67">
+      <c r="D18" s="62">
+        <v>50</v>
+      </c>
+      <c r="E18" s="63"/>
+      <c r="F18" s="64">
         <v>8</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="52">
         <v>11</v>
       </c>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54">
+      <c r="H18" s="52"/>
+      <c r="I18" s="52">
         <v>3</v>
       </c>
-      <c r="J18" s="54">
+      <c r="J18" s="52">
         <v>9</v>
       </c>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="54"/>
-      <c r="N18" s="54"/>
-      <c r="O18" s="54"/>
-      <c r="P18" s="54"/>
-      <c r="Q18" s="54"/>
-      <c r="R18" s="54"/>
-      <c r="S18" s="55"/>
-      <c r="T18" s="55"/>
-      <c r="U18" s="55"/>
-      <c r="V18" s="56">
+      <c r="K18" s="52">
+        <v>6</v>
+      </c>
+      <c r="L18" s="52">
+        <v>20</v>
+      </c>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="53"/>
+      <c r="T18" s="53"/>
+      <c r="U18" s="53"/>
+      <c r="V18" s="54">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A19" s="68" t="s">
+      <c r="A19" s="65" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="69" t="s">
+      <c r="B19" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="70">
+      <c r="C19" s="67">
         <v>60</v>
       </c>
-      <c r="D19" s="70"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="72"/>
-      <c r="H19" s="72"/>
-      <c r="I19" s="72"/>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="73"/>
-      <c r="O19" s="72"/>
-      <c r="P19" s="72"/>
-      <c r="Q19" s="72"/>
-      <c r="R19" s="72"/>
-      <c r="S19" s="74"/>
-      <c r="T19" s="74"/>
-      <c r="U19" s="74"/>
-      <c r="V19" s="75">
+      <c r="D19" s="67">
+        <v>50</v>
+      </c>
+      <c r="E19" s="67"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69">
+        <v>70</v>
+      </c>
+      <c r="M19" s="69"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+      <c r="R19" s="69"/>
+      <c r="S19" s="71"/>
+      <c r="T19" s="71"/>
+      <c r="U19" s="71"/>
+      <c r="V19" s="72">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:22">
@@ -2084,7 +2221,8 @@
       <c r="N23" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
@@ -2124,13 +2262,13 @@
     <row r="1" spans="1:22" ht="15" customHeight="1">
       <c r="A1" s="7"/>
       <c r="B1" s="8"/>
-      <c r="C1" s="87" t="s">
+      <c r="C1" s="84" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="90" t="s">
+      <c r="D1" s="87" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="89" t="s">
+      <c r="E1" s="86" t="s">
         <v>44</v>
       </c>
       <c r="F1" s="8"/>
@@ -2144,23 +2282,23 @@
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
-      <c r="Q1" s="85" t="s">
+      <c r="Q1" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="83" t="s">
+      <c r="R1" s="82"/>
+      <c r="S1" s="82"/>
+      <c r="T1" s="82"/>
+      <c r="U1" s="82"/>
+      <c r="V1" s="80" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="69.75" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="34"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="90"/>
-      <c r="E2" s="89"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="86"/>
       <c r="F2" s="34"/>
       <c r="G2" s="34"/>
       <c r="H2" s="34"/>
@@ -2172,12 +2310,12 @@
       <c r="N2" s="34"/>
       <c r="O2" s="34"/>
       <c r="P2" s="34"/>
-      <c r="Q2" s="86"/>
-      <c r="R2" s="86"/>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="84"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="81"/>
     </row>
     <row r="3" spans="1:22" ht="15.75" thickBot="1">
       <c r="A3" s="10" t="s">

</xml_diff>